<commit_message>
Simplify the solution and add comments
</commit_message>
<xml_diff>
--- a/Source/SampleRTDServer/Sample.xlsx
+++ b/Source/SampleRTDServer/Sample.xlsx
@@ -12,17 +12,14 @@
     <sheet name="גיליון3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">גיליון1!$A$5:$F$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">גיליון1!$A$5:$D$10</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
-  <si>
-    <t>RefreshRate</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Offset</t>
   </si>
@@ -31,9 +28,6 @@
   </si>
   <si>
     <t>Location</t>
-  </si>
-  <si>
-    <t>Prevtime</t>
   </si>
   <si>
     <t>local time</t>
@@ -106,56 +100,51 @@
   <volType type="realTimeData">
     <main first="samplertdserver">
       <tp t="s">
-        <v>Offset,Location,Local Time,PrevTime</v>
+        <v>Offset,Location,Local Time</v>
         <stp/>
         <stp>-help</stp>
         <stp>time</stp>
         <tr r="I16" s="1"/>
       </tp>
       <tp t="s">
-        <v>3/9/2015 12:52:58 AM</v>
+        <v>3/9/2015 1:12:49 PM</v>
         <stp/>
         <stp>time</stp>
         <stp>4</stp>
         <stp>local time</stp>
-        <tr r="F9" s="1"/>
         <tr r="D9" s="1"/>
       </tp>
       <tp t="s">
-        <v>3/9/2015 10:22:58 AM</v>
+        <v>3/9/2015 10:42:49 PM</v>
         <stp/>
         <stp>time</stp>
         <stp>5</stp>
         <stp>local time</stp>
-        <tr r="F10" s="1"/>
         <tr r="D10" s="1"/>
       </tp>
       <tp t="s">
-        <v>3/9/2015 1:22:58 AM</v>
+        <v>3/9/2015 1:42:49 PM</v>
         <stp/>
         <stp>time</stp>
         <stp>2</stp>
         <stp>local time</stp>
         <tr r="D7" s="1"/>
-        <tr r="F7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>3/8/2015 8:22:58 PM</v>
+      </tp>
+      <tp t="s">
+        <v>3/9/2015 8:42:49 AM</v>
         <stp/>
         <stp>time</stp>
         <stp>3</stp>
         <stp>local time</stp>
         <tr r="D8" s="1"/>
-        <tr r="F8" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>3/8/2015 8:22:58 AM</v>
+      </tp>
+      <tp t="s">
+        <v>3/8/2015 8:42:49 PM</v>
         <stp/>
         <stp>time</stp>
         <stp>1</stp>
         <stp>local time</stp>
         <tr r="D6" s="1"/>
-        <tr r="F6" s="1"/>
       </tp>
       <tp t="s">
         <v>-HELP,TIME</v>
@@ -242,86 +231,6 @@
         <stp>2</stp>
         <stp>Location</stp>
         <tr r="B7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>3/8/2015 8:22:57 AM</v>
-        <stp/>
-        <stp>time</stp>
-        <stp>1</stp>
-        <stp>Prevtime</stp>
-        <tr r="E6" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>3/8/2015 8:22:57 AM</v>
-        <stp/>
-        <stp>time</stp>
-        <stp>1</stp>
-        <stp>PrevTime</stp>
-        <tr r="F6" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>3/8/2015 8:22:57 PM</v>
-        <stp/>
-        <stp>time</stp>
-        <stp>3</stp>
-        <stp>Prevtime</stp>
-        <tr r="E8" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>3/8/2015 8:22:57 PM</v>
-        <stp/>
-        <stp>time</stp>
-        <stp>3</stp>
-        <stp>PrevTime</stp>
-        <tr r="F8" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>3/9/2015 1:22:57 AM</v>
-        <stp/>
-        <stp>time</stp>
-        <stp>2</stp>
-        <stp>Prevtime</stp>
-        <tr r="E7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>3/9/2015 1:22:57 AM</v>
-        <stp/>
-        <stp>time</stp>
-        <stp>2</stp>
-        <stp>PrevTime</stp>
-        <tr r="F7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>3/9/2015 10:22:57 AM</v>
-        <stp/>
-        <stp>time</stp>
-        <stp>5</stp>
-        <stp>Prevtime</stp>
-        <tr r="E10" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>3/9/2015 10:22:57 AM</v>
-        <stp/>
-        <stp>time</stp>
-        <stp>5</stp>
-        <stp>PrevTime</stp>
-        <tr r="F10" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>3/9/2015 12:52:57 AM</v>
-        <stp/>
-        <stp>time</stp>
-        <stp>4</stp>
-        <stp>Prevtime</stp>
-        <tr r="E9" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>3/9/2015 12:52:57 AM</v>
-        <stp/>
-        <stp>time</stp>
-        <stp>4</stp>
-        <stp>PrevTime</stp>
-        <tr r="F9" s="1"/>
       </tp>
     </main>
   </volType>
@@ -615,11 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,63 +542,51 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <f>SUBTOTAL(9,C6:C65001)</f>
-        <v>810</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <f>SUBTOTAL(1,C6:C65001)</f>
-        <v>202.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -704,16 +600,9 @@
       </c>
       <c r="D6" t="str">
         <f>RTD("samplertdserver",,"time",$A6,D$5)</f>
-        <v>3/8/2015 8:22:58 AM</v>
-      </c>
-      <c r="E6" t="str">
-        <f>RTD("samplertdserver",,"time",$A6,E$5)</f>
-        <v>3/8/2015 8:22:57 AM</v>
-      </c>
-      <c r="F6" s="1">
-        <f>TIMEVALUE(RTD("samplertdserver",,"time",A6,"local time"))-TIMEVALUE( RTD("samplertdserver",,"time",A6,"PrevTime"))</f>
-        <v>1.1574069503694773E-5</v>
-      </c>
+        <v>3/8/2015 8:42:49 PM</v>
+      </c>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -729,16 +618,9 @@
       </c>
       <c r="D7" t="str">
         <f>RTD("samplertdserver",,"time",$A7,D$5)</f>
-        <v>3/9/2015 1:22:58 AM</v>
-      </c>
-      <c r="E7" t="str">
-        <f>RTD("samplertdserver",,"time",$A7,E$5)</f>
-        <v>3/9/2015 1:22:57 AM</v>
-      </c>
-      <c r="F7" s="1">
-        <f>TIMEVALUE(RTD("samplertdserver",,"time",A7,"local time"))-TIMEVALUE( RTD("samplertdserver",,"time",A7,"PrevTime"))</f>
-        <v>1.1574076779652387E-5</v>
-      </c>
+        <v>3/9/2015 1:42:49 PM</v>
+      </c>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -754,16 +636,9 @@
       </c>
       <c r="D8" t="str">
         <f>RTD("samplertdserver",,"time",$A8,D$5)</f>
-        <v>3/8/2015 8:22:58 PM</v>
-      </c>
-      <c r="E8" t="str">
-        <f>RTD("samplertdserver",,"time",$A8,E$5)</f>
-        <v>3/8/2015 8:22:57 PM</v>
-      </c>
-      <c r="F8" s="1">
-        <f>TIMEVALUE(RTD("samplertdserver",,"time",A8,"local time"))-TIMEVALUE( RTD("samplertdserver",,"time",A8,"PrevTime"))</f>
-        <v>1.1574069503694773E-5</v>
-      </c>
+        <v>3/9/2015 8:42:49 AM</v>
+      </c>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -779,16 +654,9 @@
       </c>
       <c r="D9" t="str">
         <f>RTD("samplertdserver",,"time",$A9,D$5)</f>
-        <v>3/9/2015 12:52:58 AM</v>
-      </c>
-      <c r="E9" t="str">
-        <f>RTD("samplertdserver",,"time",$A9,E$5)</f>
-        <v>3/9/2015 12:52:57 AM</v>
-      </c>
-      <c r="F9" s="1">
-        <f>TIMEVALUE(RTD("samplertdserver",,"time",A9,"local time"))-TIMEVALUE( RTD("samplertdserver",,"time",A9,"PrevTime"))</f>
-        <v>1.1574069503694773E-5</v>
-      </c>
+        <v>3/9/2015 1:12:49 PM</v>
+      </c>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -804,16 +672,9 @@
       </c>
       <c r="D10" t="str">
         <f>RTD("samplertdserver",,"time",$A10,D$5)</f>
-        <v>3/9/2015 10:22:58 AM</v>
-      </c>
-      <c r="E10" t="str">
-        <f>RTD("samplertdserver",,"time",$A10,E$5)</f>
-        <v>3/9/2015 10:22:57 AM</v>
-      </c>
-      <c r="F10" s="1">
-        <f>TIMEVALUE(RTD("samplertdserver",,"time",A10,"local time"))-TIMEVALUE( RTD("samplertdserver",,"time",A10,"PrevTime"))</f>
-        <v>1.1574076779652387E-5</v>
-      </c>
+        <v>3/9/2015 10:42:49 PM</v>
+      </c>
+      <c r="F10" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I15" t="str">
@@ -824,20 +685,11 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I16" t="str">
         <f>RTD("samplertdserver",,"-help","time")</f>
-        <v>Offset,Location,Local Time,PrevTime</v>
+        <v>Offset,Location,Local Time</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A5:F10">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="0"/>
-        <filter val="270"/>
-        <filter val="-300"/>
-        <filter val="840"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A5:D10"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>